<commit_message>
First cut of moving to generated loans. Tests don't pass
</commit_message>
<xml_diff>
--- a/YoFi.Tests/SampleData/TestData1.xlsx
+++ b/YoFi.Tests/SampleData/TestData1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\jcoliz\Ofx\YoFi.Tests\SampleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C497EC-4D64-4D50-96AB-EC087B4AE4C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4332DA1-085C-4971-9BA7-6D778AA1B6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10110" yWindow="2730" windowWidth="28800" windowHeight="15460" xr2:uid="{D78380F0-A539-4D8B-9BEC-B3C0621EF4A6}"/>
+    <workbookView xWindow="2610" yWindow="3760" windowWidth="24420" windowHeight="15460" xr2:uid="{D78380F0-A539-4D8B-9BEC-B3C0621EF4A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Definition" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="70">
-  <si>
-    <t>Housing:Mortgage Interest</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="71">
   <si>
     <t>Housing:Property Tax</t>
   </si>
@@ -244,6 +241,12 @@
   </si>
   <si>
     <t>DateRepeats</t>
+  </si>
+  <si>
+    <t>Loan</t>
+  </si>
+  <si>
+    <t>{ "interest": "Housing: Mortgage Interest", "amount": 375000, "rate": 3, "term": 360, "origination": "1/1/2010" }</t>
   </si>
 </sst>
 </file>
@@ -333,9 +336,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1E37678C-2EAF-4E37-B1FA-AD78BDAEE85C}" name="Table1" displayName="Table1" ref="A1:H33" totalsRowShown="0">
-  <autoFilter ref="A1:H33" xr:uid="{1E37678C-2EAF-4E37-B1FA-AD78BDAEE85C}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1E37678C-2EAF-4E37-B1FA-AD78BDAEE85C}" name="Table1" displayName="Table1" ref="A1:I32" totalsRowShown="0">
+  <autoFilter ref="A1:I32" xr:uid="{1E37678C-2EAF-4E37-B1FA-AD78BDAEE85C}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{2D305D92-F06E-4A42-ADD5-8905CE687361}" name="Category"/>
     <tableColumn id="2" xr3:uid="{CD6746BA-7D2E-459B-9C57-966F0DD88C48}" name="Payee"/>
     <tableColumn id="3" xr3:uid="{93117429-1FD4-4AA7-BE38-B0D0B1C52453}" name="AmountYearly" dataDxfId="0" dataCellStyle="Currency"/>
@@ -344,6 +347,7 @@
     <tableColumn id="5" xr3:uid="{778F6780-87B7-466A-8305-1DFBFB539DA5}" name="AmountJitter"/>
     <tableColumn id="6" xr3:uid="{57ACD242-AF26-46E4-AC6D-23DE7A7410EC}" name="DateJitter"/>
     <tableColumn id="15" xr3:uid="{A48EA1D1-3BF2-427F-B68E-F650AE4C5A46}" name="Group"/>
+    <tableColumn id="8" xr3:uid="{3203CD1C-FA1C-4558-8149-BA42D96D4BC7}" name="Loan"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -646,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BFC0386-6A87-4615-9CF7-243BB5DCA6C5}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -661,110 +665,117 @@
     <col min="5" max="5" width="13.81640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.08984375" customWidth="1"/>
     <col min="7" max="8" width="11.26953125" customWidth="1"/>
+    <col min="9" max="9" width="94.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" t="s">
-        <v>40</v>
-      </c>
       <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
         <v>67</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>68</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" t="s">
         <v>69</v>
       </c>
-      <c r="F1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="1">
-        <f>-800*12</f>
-        <v>-9600</v>
+        <f>-1581.02*12</f>
+        <v>-18972.239999999998</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+      <c r="I2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
       </c>
       <c r="C3" s="1">
-        <f>-700*12</f>
-        <v>-8400</v>
+        <f>-400</f>
+        <v>-400</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C4" s="1">
-        <f>-400</f>
-        <v>-400</v>
+        <f>-5000</f>
+        <v>-5000</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="C5" s="1">
-        <f>-5000</f>
-        <v>-5000</v>
+        <f>-300*12</f>
+        <v>-3600</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -773,262 +784,262 @@
         <v>9</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C6" s="1">
-        <f>-300*12</f>
-        <v>-3600</v>
+        <f>-75*12</f>
+        <v>-900</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="1">
-        <f>-75*12</f>
-        <v>-900</v>
+        <f>-50*12</f>
+        <v>-600</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="C8" s="1">
-        <f>-50*12</f>
-        <v>-600</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="1">
         <f>-350*52</f>
         <v>-18200</v>
       </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" t="s">
         <v>10</v>
       </c>
-      <c r="G9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" s="1">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="1">
         <f>-52*3*50</f>
         <v>-7800</v>
       </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10">
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9">
         <v>3</v>
       </c>
-      <c r="F10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="1">
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="1">
         <f>-1200</f>
         <v>-1200</v>
       </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="1">
+        <f>-150*12</f>
+        <v>-1800</v>
+      </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C12" s="1">
-        <f>-150*12</f>
-        <v>-1800</v>
+        <f>-40*6</f>
+        <v>-240</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C13" s="1">
-        <f>-40*6</f>
-        <v>-240</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="1">
         <f>-250</f>
         <v>-250</v>
       </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="1">
+        <f>52*-35</f>
+        <v>-1820</v>
+      </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C15" s="1">
-        <f>52*-35</f>
-        <v>-1820</v>
-      </c>
-      <c r="D15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="1">
         <f>-500</f>
         <v>-500</v>
       </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="1">
+        <f>-300</f>
+        <v>-300</v>
+      </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
         <v>50</v>
       </c>
       <c r="C17" s="1">
-        <f>-300</f>
-        <v>-300</v>
+        <f>-400*12</f>
+        <v>-4800</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F17" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -1039,17 +1050,17 @@
         <v>51</v>
       </c>
       <c r="C18" s="1">
-        <f>-400*12</f>
-        <v>-4800</v>
+        <f>-2000</f>
+        <v>-2000</v>
       </c>
       <c r="D18" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F18" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G18" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -1057,20 +1068,20 @@
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C19" s="1">
-        <f>-2000</f>
-        <v>-2000</v>
+        <f>-25*12</f>
+        <v>-300</v>
       </c>
       <c r="D19" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F19" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -1078,20 +1089,20 @@
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C20" s="1">
-        <f>-25*12</f>
-        <v>-300</v>
+        <f>-125*4</f>
+        <v>-500</v>
       </c>
       <c r="D20" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G20" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -1099,85 +1110,85 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C21" s="1">
-        <f>-125*4</f>
-        <v>-500</v>
+        <v>120000</v>
       </c>
       <c r="D21" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="F21" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G21" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="H21" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="C22" s="1">
-        <v>120000</v>
+        <f>4000</f>
+        <v>4000</v>
       </c>
       <c r="D22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G22" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C23" s="1">
-        <f>4000</f>
-        <v>4000</v>
+        <f>-687*24</f>
+        <v>-16488</v>
       </c>
       <c r="D23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C24" s="1">
-        <f>-687*24</f>
-        <v>-16488</v>
+        <f>-310*24</f>
+        <v>-7440</v>
       </c>
       <c r="D24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -1185,41 +1196,41 @@
         <v>25</v>
       </c>
       <c r="C25" s="1">
-        <f>-310*24</f>
-        <v>-7440</v>
+        <f>-73*24</f>
+        <v>-1752</v>
       </c>
       <c r="D25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="1">
+        <f>-260*24</f>
+        <v>-6240</v>
+      </c>
+      <c r="D26" t="s">
+        <v>60</v>
+      </c>
+      <c r="F26" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" t="s">
         <v>26</v>
-      </c>
-      <c r="C26" s="1">
-        <f>-73*24</f>
-        <v>-1752</v>
-      </c>
-      <c r="D26" t="s">
-        <v>61</v>
-      </c>
-      <c r="F26" t="s">
-        <v>9</v>
-      </c>
-      <c r="G26" t="s">
-        <v>9</v>
-      </c>
-      <c r="H26" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -1227,62 +1238,62 @@
         <v>34</v>
       </c>
       <c r="C27" s="1">
-        <f>-260*24</f>
-        <v>-6240</v>
+        <f>-48*24</f>
+        <v>-1152</v>
       </c>
       <c r="D27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="C28" s="1">
-        <f>-48*24</f>
-        <v>-1152</v>
+        <f>-500*12</f>
+        <v>-6000</v>
       </c>
       <c r="D28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C29" s="1">
-        <f>-500*12</f>
-        <v>-6000</v>
+        <f>-4000</f>
+        <v>-4000</v>
       </c>
       <c r="D29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
@@ -1290,41 +1301,41 @@
         <v>29</v>
       </c>
       <c r="C30" s="1">
-        <f>-4000</f>
-        <v>-4000</v>
+        <f>-19000</f>
+        <v>-19000</v>
       </c>
       <c r="D30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C31" s="1">
-        <f>-19000</f>
-        <v>-19000</v>
+        <f>-200</f>
+        <v>-200</v>
       </c>
       <c r="D31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -1332,41 +1343,20 @@
         <v>16</v>
       </c>
       <c r="C32" s="1">
-        <f>-200</f>
-        <v>-200</v>
-      </c>
-      <c r="D32" t="s">
-        <v>61</v>
-      </c>
-      <c r="F32" t="s">
-        <v>9</v>
-      </c>
-      <c r="G32" t="s">
-        <v>9</v>
-      </c>
-      <c r="H32" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" s="1">
         <f>-50</f>
         <v>-50</v>
       </c>
-      <c r="D33" t="s">
-        <v>61</v>
-      </c>
-      <c r="F33" t="s">
-        <v>9</v>
-      </c>
-      <c r="G33" t="s">
-        <v>9</v>
-      </c>
-      <c r="H33" t="s">
-        <v>27</v>
+      <c r="D32" t="s">
+        <v>60</v>
+      </c>
+      <c r="F32" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>